<commit_message>
updated algorithm and stats on findings
</commit_message>
<xml_diff>
--- a/datasets/performance-analysis.xlsx
+++ b/datasets/performance-analysis.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julkroll/Documents/jk/grad-ms/fall2020-courses/computer-vision/cv-final-project/joynuelle.github.io-cs639/Datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JoyNuelle/Desktop/cs639/final_project/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1410454A-DF6D-A54B-BD77-357112D325D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8950A17A-6CCF-0148-B012-E643C310DC39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" activeTab="1" xr2:uid="{25C92B33-322F-9E48-B40C-C9A6D0D7FB01}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19520" windowHeight="15980" activeTab="1" xr2:uid="{25C92B33-322F-9E48-B40C-C9A6D0D7FB01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
   <si>
     <t>Joy</t>
   </si>
@@ -77,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -105,6 +106,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -136,13 +149,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +476,7 @@
   <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="A1:M1048576"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2452,10 +2468,2021 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FAFDA21-5613-1146-954D-C5508723246E}">
+  <dimension ref="A1:P53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>31</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2" s="7">
+        <v>27</v>
+      </c>
+      <c r="H2">
+        <v>8102</v>
+      </c>
+      <c r="I2" s="1">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1">
+        <v>6</v>
+      </c>
+      <c r="M2" s="7">
+        <v>30</v>
+      </c>
+      <c r="O2" s="3"/>
+      <c r="P2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>37</v>
+      </c>
+      <c r="D3">
+        <v>45</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>8103</v>
+      </c>
+      <c r="I3" s="1">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1">
+        <v>4</v>
+      </c>
+      <c r="M3" s="7">
+        <v>38</v>
+      </c>
+      <c r="O3" s="7"/>
+      <c r="P3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>8104</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <v>28</v>
+      </c>
+      <c r="L4">
+        <v>11</v>
+      </c>
+      <c r="M4" s="7">
+        <v>17</v>
+      </c>
+      <c r="O4" s="5"/>
+      <c r="P4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1">
+        <v>9</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>8105</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="L5" s="1">
+        <v>9</v>
+      </c>
+      <c r="M5" s="7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>18</v>
+      </c>
+      <c r="C6">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>19</v>
+      </c>
+      <c r="F6">
+        <v>38</v>
+      </c>
+      <c r="H6">
+        <v>8106</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+      <c r="L6" s="1">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
+      </c>
+      <c r="C7">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>18</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+      <c r="H7">
+        <v>8107</v>
+      </c>
+      <c r="I7" s="1">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>24</v>
+      </c>
+      <c r="K7">
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <v>15</v>
+      </c>
+      <c r="M7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>46</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+      <c r="D8">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>34</v>
+      </c>
+      <c r="H8">
+        <v>8108</v>
+      </c>
+      <c r="I8" s="1">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>23</v>
+      </c>
+      <c r="K8">
+        <v>14</v>
+      </c>
+      <c r="L8">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>19</v>
+      </c>
+      <c r="C9">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>13</v>
+      </c>
+      <c r="E9">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>22</v>
+      </c>
+      <c r="H9">
+        <v>8109</v>
+      </c>
+      <c r="I9">
+        <v>11</v>
+      </c>
+      <c r="J9" s="1">
+        <v>5</v>
+      </c>
+      <c r="K9">
+        <v>45</v>
+      </c>
+      <c r="L9">
+        <v>17</v>
+      </c>
+      <c r="M9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>12</v>
+      </c>
+      <c r="C10">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+      <c r="E10">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10">
+        <v>8110</v>
+      </c>
+      <c r="I10">
+        <v>15</v>
+      </c>
+      <c r="J10">
+        <v>26</v>
+      </c>
+      <c r="K10">
+        <v>46</v>
+      </c>
+      <c r="L10">
+        <v>18</v>
+      </c>
+      <c r="M10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>47</v>
+      </c>
+      <c r="D11">
+        <v>39</v>
+      </c>
+      <c r="E11">
+        <v>49</v>
+      </c>
+      <c r="F11">
+        <v>29</v>
+      </c>
+      <c r="H11">
+        <v>8111</v>
+      </c>
+      <c r="I11">
+        <v>16</v>
+      </c>
+      <c r="J11">
+        <v>43</v>
+      </c>
+      <c r="K11">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>26</v>
+      </c>
+      <c r="M11" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>37</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>8112</v>
+      </c>
+      <c r="I12">
+        <v>18</v>
+      </c>
+      <c r="J12">
+        <v>47</v>
+      </c>
+      <c r="K12">
+        <v>20</v>
+      </c>
+      <c r="L12">
+        <v>25</v>
+      </c>
+      <c r="M12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
+      </c>
+      <c r="E13" s="1">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>8113</v>
+      </c>
+      <c r="I13" s="1">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>16</v>
+      </c>
+      <c r="K13">
+        <v>11</v>
+      </c>
+      <c r="L13">
+        <v>28</v>
+      </c>
+      <c r="M13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>49</v>
+      </c>
+      <c r="C14">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>37</v>
+      </c>
+      <c r="E14">
+        <v>44</v>
+      </c>
+      <c r="F14">
+        <v>13</v>
+      </c>
+      <c r="H14">
+        <v>8114</v>
+      </c>
+      <c r="I14" s="1">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8</v>
+      </c>
+      <c r="K14">
+        <v>12</v>
+      </c>
+      <c r="L14">
+        <v>22</v>
+      </c>
+      <c r="M14" s="7">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>36</v>
+      </c>
+      <c r="F15" s="7">
+        <v>11</v>
+      </c>
+      <c r="H15">
+        <v>8115</v>
+      </c>
+      <c r="I15">
+        <v>13</v>
+      </c>
+      <c r="J15" s="1">
+        <v>6</v>
+      </c>
+      <c r="K15" s="1">
+        <v>5</v>
+      </c>
+      <c r="L15">
+        <v>27</v>
+      </c>
+      <c r="M15" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>35</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>42</v>
+      </c>
+      <c r="F16">
+        <v>14</v>
+      </c>
+      <c r="H16">
+        <v>8116</v>
+      </c>
+      <c r="I16">
+        <v>14</v>
+      </c>
+      <c r="J16" s="1">
+        <v>7</v>
+      </c>
+      <c r="K16" s="1">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>21</v>
+      </c>
+      <c r="M16" s="7">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>30</v>
+      </c>
+      <c r="D17">
+        <v>29</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>43</v>
+      </c>
+      <c r="H17">
+        <v>8117</v>
+      </c>
+      <c r="I17">
+        <v>28</v>
+      </c>
+      <c r="J17">
+        <v>30</v>
+      </c>
+      <c r="K17" s="1">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>30</v>
+      </c>
+      <c r="M17" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>11</v>
+      </c>
+      <c r="C18">
+        <v>44</v>
+      </c>
+      <c r="D18">
+        <v>30</v>
+      </c>
+      <c r="E18">
+        <v>13</v>
+      </c>
+      <c r="F18">
+        <v>21</v>
+      </c>
+      <c r="H18">
+        <v>8118</v>
+      </c>
+      <c r="I18">
+        <v>25</v>
+      </c>
+      <c r="J18">
+        <v>35</v>
+      </c>
+      <c r="K18" s="1">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>29</v>
+      </c>
+      <c r="M18">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1">
+        <v>10</v>
+      </c>
+      <c r="F19" s="7">
+        <v>33</v>
+      </c>
+      <c r="H19">
+        <v>8119</v>
+      </c>
+      <c r="I19">
+        <v>27</v>
+      </c>
+      <c r="J19">
+        <v>41</v>
+      </c>
+      <c r="K19">
+        <v>47</v>
+      </c>
+      <c r="L19">
+        <v>33</v>
+      </c>
+      <c r="M19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="6">
+        <v>5</v>
+      </c>
+      <c r="H20">
+        <v>8120</v>
+      </c>
+      <c r="I20">
+        <v>26</v>
+      </c>
+      <c r="J20">
+        <v>42</v>
+      </c>
+      <c r="K20">
+        <v>48</v>
+      </c>
+      <c r="L20">
+        <v>34</v>
+      </c>
+      <c r="M20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>39</v>
+      </c>
+      <c r="D21">
+        <v>42</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>49</v>
+      </c>
+      <c r="H21">
+        <v>8121</v>
+      </c>
+      <c r="I21">
+        <v>17</v>
+      </c>
+      <c r="J21" s="1">
+        <v>3</v>
+      </c>
+      <c r="K21">
+        <v>21</v>
+      </c>
+      <c r="L21" s="1">
+        <v>8</v>
+      </c>
+      <c r="M21" s="7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>27</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
+      </c>
+      <c r="F22">
+        <v>46</v>
+      </c>
+      <c r="H22">
+        <v>8122</v>
+      </c>
+      <c r="I22">
+        <v>19</v>
+      </c>
+      <c r="J22">
+        <v>40</v>
+      </c>
+      <c r="K22">
+        <v>24</v>
+      </c>
+      <c r="L22">
+        <v>46</v>
+      </c>
+      <c r="M22">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>48</v>
+      </c>
+      <c r="C23">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>21</v>
+      </c>
+      <c r="E23">
+        <v>23</v>
+      </c>
+      <c r="F23">
+        <v>28</v>
+      </c>
+      <c r="H23">
+        <v>8123</v>
+      </c>
+      <c r="I23">
+        <v>31</v>
+      </c>
+      <c r="J23">
+        <v>36</v>
+      </c>
+      <c r="K23">
+        <v>25</v>
+      </c>
+      <c r="L23">
+        <v>45</v>
+      </c>
+      <c r="M23">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>33</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7</v>
+      </c>
+      <c r="E24">
+        <v>24</v>
+      </c>
+      <c r="F24">
+        <v>36</v>
+      </c>
+      <c r="H24">
+        <v>8124</v>
+      </c>
+      <c r="I24">
+        <v>20</v>
+      </c>
+      <c r="J24">
+        <v>44</v>
+      </c>
+      <c r="K24">
+        <v>15</v>
+      </c>
+      <c r="L24">
+        <v>32</v>
+      </c>
+      <c r="M24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25" s="1">
+        <v>5</v>
+      </c>
+      <c r="E25" s="1">
+        <v>4</v>
+      </c>
+      <c r="F25" s="2">
+        <v>9</v>
+      </c>
+      <c r="H25">
+        <v>8125</v>
+      </c>
+      <c r="I25">
+        <v>21</v>
+      </c>
+      <c r="J25">
+        <v>39</v>
+      </c>
+      <c r="K25">
+        <v>16</v>
+      </c>
+      <c r="L25">
+        <v>31</v>
+      </c>
+      <c r="M25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+      <c r="D26">
+        <v>34</v>
+      </c>
+      <c r="E26">
+        <v>35</v>
+      </c>
+      <c r="F26">
+        <v>32</v>
+      </c>
+      <c r="H26">
+        <v>8126</v>
+      </c>
+      <c r="I26">
+        <v>24</v>
+      </c>
+      <c r="J26">
+        <v>20</v>
+      </c>
+      <c r="K26">
+        <v>31</v>
+      </c>
+      <c r="L26">
+        <v>44</v>
+      </c>
+      <c r="M26">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27">
+        <v>28</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27">
+        <v>28</v>
+      </c>
+      <c r="F27">
+        <v>35</v>
+      </c>
+      <c r="H27">
+        <v>8127</v>
+      </c>
+      <c r="I27">
+        <v>36</v>
+      </c>
+      <c r="J27">
+        <v>50</v>
+      </c>
+      <c r="K27">
+        <v>32</v>
+      </c>
+      <c r="L27">
+        <v>51</v>
+      </c>
+      <c r="M27" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>23</v>
+      </c>
+      <c r="C28">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28">
+        <v>34</v>
+      </c>
+      <c r="F28">
+        <v>17</v>
+      </c>
+      <c r="H28">
+        <v>8128</v>
+      </c>
+      <c r="I28">
+        <v>30</v>
+      </c>
+      <c r="J28">
+        <v>25</v>
+      </c>
+      <c r="K28">
+        <v>33</v>
+      </c>
+      <c r="L28">
+        <v>20</v>
+      </c>
+      <c r="M28">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>24</v>
+      </c>
+      <c r="C29">
+        <v>40</v>
+      </c>
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29">
+        <v>25</v>
+      </c>
+      <c r="F29">
+        <v>47</v>
+      </c>
+      <c r="H29">
+        <v>8129</v>
+      </c>
+      <c r="I29">
+        <v>29</v>
+      </c>
+      <c r="J29">
+        <v>18</v>
+      </c>
+      <c r="K29">
+        <v>44</v>
+      </c>
+      <c r="L29">
+        <v>16</v>
+      </c>
+      <c r="M29">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>50</v>
+      </c>
+      <c r="C30">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>43</v>
+      </c>
+      <c r="E30">
+        <v>14</v>
+      </c>
+      <c r="F30">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>8130</v>
+      </c>
+      <c r="I30">
+        <v>37</v>
+      </c>
+      <c r="J30">
+        <v>48</v>
+      </c>
+      <c r="K30">
+        <v>17</v>
+      </c>
+      <c r="L30">
+        <v>42</v>
+      </c>
+      <c r="M30" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>18</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>44</v>
+      </c>
+      <c r="H31">
+        <v>8131</v>
+      </c>
+      <c r="I31">
+        <v>38</v>
+      </c>
+      <c r="J31">
+        <v>49</v>
+      </c>
+      <c r="K31">
+        <v>18</v>
+      </c>
+      <c r="L31">
+        <v>43</v>
+      </c>
+      <c r="M31">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>37</v>
+      </c>
+      <c r="C32">
+        <v>36</v>
+      </c>
+      <c r="D32">
+        <v>47</v>
+      </c>
+      <c r="E32">
+        <v>16</v>
+      </c>
+      <c r="F32">
+        <v>23</v>
+      </c>
+      <c r="H32">
+        <v>8132</v>
+      </c>
+      <c r="I32">
+        <v>23</v>
+      </c>
+      <c r="J32">
+        <v>19</v>
+      </c>
+      <c r="K32">
+        <v>22</v>
+      </c>
+      <c r="L32" s="1">
+        <v>10</v>
+      </c>
+      <c r="M32">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>25</v>
+      </c>
+      <c r="C33">
+        <v>24</v>
+      </c>
+      <c r="D33">
+        <v>25</v>
+      </c>
+      <c r="E33">
+        <v>29</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+      <c r="H33">
+        <v>8133</v>
+      </c>
+      <c r="I33">
+        <v>22</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+      <c r="K33">
+        <v>23</v>
+      </c>
+      <c r="L33">
+        <v>7</v>
+      </c>
+      <c r="M33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>26</v>
+      </c>
+      <c r="C34">
+        <v>25</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9</v>
+      </c>
+      <c r="E34">
+        <v>27</v>
+      </c>
+      <c r="F34">
+        <v>39</v>
+      </c>
+      <c r="H34">
+        <v>8134</v>
+      </c>
+      <c r="I34" s="1">
+        <v>5</v>
+      </c>
+      <c r="J34" s="1">
+        <v>2</v>
+      </c>
+      <c r="K34" s="1">
+        <v>1</v>
+      </c>
+      <c r="L34" s="1">
+        <v>3</v>
+      </c>
+      <c r="M34" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>35</v>
+      </c>
+      <c r="C35" s="1">
+        <v>8</v>
+      </c>
+      <c r="D35">
+        <v>12</v>
+      </c>
+      <c r="E35" s="1">
+        <v>8</v>
+      </c>
+      <c r="F35" s="8">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>8135</v>
+      </c>
+      <c r="I35" s="1">
+        <v>6</v>
+      </c>
+      <c r="J35" s="1">
+        <v>1</v>
+      </c>
+      <c r="K35" s="1">
+        <v>2</v>
+      </c>
+      <c r="L35" s="1">
+        <v>1</v>
+      </c>
+      <c r="M35" s="7">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>26</v>
+      </c>
+      <c r="E36" s="1">
+        <v>7</v>
+      </c>
+      <c r="F36" s="7">
+        <v>31</v>
+      </c>
+      <c r="H36">
+        <v>8136</v>
+      </c>
+      <c r="I36">
+        <v>39</v>
+      </c>
+      <c r="J36">
+        <v>38</v>
+      </c>
+      <c r="K36" s="1">
+        <v>9</v>
+      </c>
+      <c r="L36">
+        <v>24</v>
+      </c>
+      <c r="M36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>45</v>
+      </c>
+      <c r="C37">
+        <v>42</v>
+      </c>
+      <c r="D37">
+        <v>38</v>
+      </c>
+      <c r="E37">
+        <v>46</v>
+      </c>
+      <c r="F37">
+        <v>19</v>
+      </c>
+      <c r="H37">
+        <v>8137</v>
+      </c>
+      <c r="I37">
+        <v>40</v>
+      </c>
+      <c r="J37">
+        <v>31</v>
+      </c>
+      <c r="K37" s="1">
+        <v>10</v>
+      </c>
+      <c r="L37">
+        <v>23</v>
+      </c>
+      <c r="M37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>32</v>
+      </c>
+      <c r="C38">
+        <v>19</v>
+      </c>
+      <c r="D38" s="1">
+        <v>6</v>
+      </c>
+      <c r="E38" s="1">
+        <v>2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>8138</v>
+      </c>
+      <c r="I38">
+        <v>48</v>
+      </c>
+      <c r="J38" s="1">
+        <v>10</v>
+      </c>
+      <c r="K38">
+        <v>41</v>
+      </c>
+      <c r="L38" s="1">
+        <v>5</v>
+      </c>
+      <c r="M38" s="7">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>39</v>
+      </c>
+      <c r="C39">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>48</v>
+      </c>
+      <c r="E39">
+        <v>45</v>
+      </c>
+      <c r="F39">
+        <v>20</v>
+      </c>
+      <c r="H39">
+        <v>8139</v>
+      </c>
+      <c r="I39">
+        <v>49</v>
+      </c>
+      <c r="J39">
+        <v>34</v>
+      </c>
+      <c r="K39">
+        <v>49</v>
+      </c>
+      <c r="L39">
+        <v>47</v>
+      </c>
+      <c r="M39">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="C40">
+        <v>49</v>
+      </c>
+      <c r="D40">
+        <v>44</v>
+      </c>
+      <c r="E40">
+        <v>48</v>
+      </c>
+      <c r="F40">
+        <v>48</v>
+      </c>
+      <c r="H40">
+        <v>8140</v>
+      </c>
+      <c r="I40">
+        <v>41</v>
+      </c>
+      <c r="J40">
+        <v>33</v>
+      </c>
+      <c r="K40">
+        <v>42</v>
+      </c>
+      <c r="L40">
+        <v>36</v>
+      </c>
+      <c r="M40">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>23</v>
+      </c>
+      <c r="D41">
+        <v>19</v>
+      </c>
+      <c r="E41">
+        <v>39</v>
+      </c>
+      <c r="F41">
+        <v>15</v>
+      </c>
+      <c r="H41">
+        <v>8141</v>
+      </c>
+      <c r="I41">
+        <v>42</v>
+      </c>
+      <c r="J41">
+        <v>51</v>
+      </c>
+      <c r="K41">
+        <v>43</v>
+      </c>
+      <c r="L41">
+        <v>37</v>
+      </c>
+      <c r="M41">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>21</v>
+      </c>
+      <c r="C42">
+        <v>32</v>
+      </c>
+      <c r="D42">
+        <v>35</v>
+      </c>
+      <c r="E42">
+        <v>26</v>
+      </c>
+      <c r="F42">
+        <v>16</v>
+      </c>
+      <c r="H42">
+        <v>8142</v>
+      </c>
+      <c r="I42">
+        <v>47</v>
+      </c>
+      <c r="J42">
+        <v>15</v>
+      </c>
+      <c r="K42">
+        <v>34</v>
+      </c>
+      <c r="L42">
+        <v>41</v>
+      </c>
+      <c r="M42" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>36</v>
+      </c>
+      <c r="C43" s="1">
+        <v>4</v>
+      </c>
+      <c r="D43">
+        <v>11</v>
+      </c>
+      <c r="E43" s="1">
+        <v>6</v>
+      </c>
+      <c r="F43" s="2">
+        <v>3</v>
+      </c>
+      <c r="H43">
+        <v>8143</v>
+      </c>
+      <c r="I43">
+        <v>44</v>
+      </c>
+      <c r="J43">
+        <v>29</v>
+      </c>
+      <c r="K43">
+        <v>35</v>
+      </c>
+      <c r="L43">
+        <v>40</v>
+      </c>
+      <c r="M43">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+      <c r="D44">
+        <v>22</v>
+      </c>
+      <c r="E44">
+        <v>32</v>
+      </c>
+      <c r="F44">
+        <v>41</v>
+      </c>
+      <c r="H44">
+        <v>8144</v>
+      </c>
+      <c r="I44">
+        <v>33</v>
+      </c>
+      <c r="J44">
+        <v>37</v>
+      </c>
+      <c r="K44" s="1">
+        <v>3</v>
+      </c>
+      <c r="L44">
+        <v>14</v>
+      </c>
+      <c r="M44" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>27</v>
+      </c>
+      <c r="C45" s="1">
+        <v>5</v>
+      </c>
+      <c r="D45">
+        <v>49</v>
+      </c>
+      <c r="E45">
+        <v>33</v>
+      </c>
+      <c r="F45">
+        <v>12</v>
+      </c>
+      <c r="H45">
+        <v>8145</v>
+      </c>
+      <c r="I45">
+        <v>34</v>
+      </c>
+      <c r="J45">
+        <v>17</v>
+      </c>
+      <c r="K45" s="1">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>13</v>
+      </c>
+      <c r="M45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>38</v>
+      </c>
+      <c r="C46">
+        <v>46</v>
+      </c>
+      <c r="D46">
+        <v>40</v>
+      </c>
+      <c r="E46">
+        <v>43</v>
+      </c>
+      <c r="F46">
+        <v>50</v>
+      </c>
+      <c r="H46">
+        <v>8146</v>
+      </c>
+      <c r="I46">
+        <v>43</v>
+      </c>
+      <c r="J46">
+        <v>32</v>
+      </c>
+      <c r="K46">
+        <v>36</v>
+      </c>
+      <c r="L46">
+        <v>38</v>
+      </c>
+      <c r="M46">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47">
+        <v>45</v>
+      </c>
+      <c r="D47">
+        <v>41</v>
+      </c>
+      <c r="E47">
+        <v>50</v>
+      </c>
+      <c r="F47">
+        <v>45</v>
+      </c>
+      <c r="H47">
+        <v>8147</v>
+      </c>
+      <c r="I47">
+        <v>35</v>
+      </c>
+      <c r="J47">
+        <v>27</v>
+      </c>
+      <c r="K47">
+        <v>37</v>
+      </c>
+      <c r="L47">
+        <v>35</v>
+      </c>
+      <c r="M47">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>41</v>
+      </c>
+      <c r="C48">
+        <v>13</v>
+      </c>
+      <c r="D48">
+        <v>32</v>
+      </c>
+      <c r="E48">
+        <v>38</v>
+      </c>
+      <c r="F48">
+        <v>26</v>
+      </c>
+      <c r="H48">
+        <v>8148</v>
+      </c>
+      <c r="I48">
+        <v>45</v>
+      </c>
+      <c r="J48">
+        <v>21</v>
+      </c>
+      <c r="K48">
+        <v>38</v>
+      </c>
+      <c r="L48">
+        <v>48</v>
+      </c>
+      <c r="M48" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>29</v>
+      </c>
+      <c r="C49" s="1">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>33</v>
+      </c>
+      <c r="E49">
+        <v>40</v>
+      </c>
+      <c r="F49">
+        <v>42</v>
+      </c>
+      <c r="H49">
+        <v>8149</v>
+      </c>
+      <c r="I49">
+        <v>46</v>
+      </c>
+      <c r="J49">
+        <v>22</v>
+      </c>
+      <c r="K49">
+        <v>39</v>
+      </c>
+      <c r="L49">
+        <v>39</v>
+      </c>
+      <c r="M49">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>34</v>
+      </c>
+      <c r="C50">
+        <v>31</v>
+      </c>
+      <c r="D50">
+        <v>36</v>
+      </c>
+      <c r="E50">
+        <v>41</v>
+      </c>
+      <c r="F50">
+        <v>30</v>
+      </c>
+      <c r="H50">
+        <v>8150</v>
+      </c>
+      <c r="I50">
+        <v>32</v>
+      </c>
+      <c r="J50">
+        <v>28</v>
+      </c>
+      <c r="K50">
+        <v>40</v>
+      </c>
+      <c r="L50">
+        <v>19</v>
+      </c>
+      <c r="M50">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>43</v>
+      </c>
+      <c r="C51">
+        <v>12</v>
+      </c>
+      <c r="D51">
+        <v>23</v>
+      </c>
+      <c r="E51">
+        <v>31</v>
+      </c>
+      <c r="F51">
+        <v>24</v>
+      </c>
+      <c r="H51">
+        <v>8151</v>
+      </c>
+      <c r="I51">
+        <v>50</v>
+      </c>
+      <c r="J51">
+        <v>52</v>
+      </c>
+      <c r="K51">
+        <v>50</v>
+      </c>
+      <c r="L51">
+        <v>49</v>
+      </c>
+      <c r="M51">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <v>8152</v>
+      </c>
+      <c r="I52">
+        <v>51</v>
+      </c>
+      <c r="J52">
+        <v>46</v>
+      </c>
+      <c r="K52">
+        <v>51</v>
+      </c>
+      <c r="L52">
+        <v>52</v>
+      </c>
+      <c r="M52">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <v>8153</v>
+      </c>
+      <c r="I53">
+        <v>52</v>
+      </c>
+      <c r="J53">
+        <v>45</v>
+      </c>
+      <c r="K53">
+        <v>52</v>
+      </c>
+      <c r="L53">
+        <v>50</v>
+      </c>
+      <c r="M53">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA9403D5-4D35-D048-B06A-603AF6C84E1D}">
   <dimension ref="A1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2836,10 +4863,10 @@
         <v>22</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E10">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3">
         <v>4</v>

</xml_diff>